<commit_message>
updates respirometry and notebook
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24500" windowHeight="15360" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="24260" windowHeight="15120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="224">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -637,6 +637,63 @@
   </si>
   <si>
     <t>11:30</t>
+  </si>
+  <si>
+    <t>2017-11-04</t>
+  </si>
+  <si>
+    <t>18:50</t>
+  </si>
+  <si>
+    <t>2017-11-02</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apple </t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fly </t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>2017-11-05</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>2017-11-07</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>2017-11-08</t>
+  </si>
+  <si>
+    <t>71</t>
   </si>
 </sst>
 </file>
@@ -1345,13 +1402,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W137"/>
+  <dimension ref="A1:W146"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D106" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D121" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K128" sqref="K128"/>
+      <selection pane="bottomRight" activeCell="J146" sqref="J146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4724,6 +4781,12 @@
       <c r="M126" s="1" t="s">
         <v>201</v>
       </c>
+      <c r="N126" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="O126" s="1" t="s">
+        <v>206</v>
+      </c>
       <c r="P126" s="1" t="s">
         <v>171</v>
       </c>
@@ -5013,23 +5076,341 @@
       </c>
     </row>
     <row r="134" spans="1:16">
+      <c r="A134" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="I134" s="1" t="s">
         <v>164</v>
       </c>
+      <c r="J134" s="1" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="135" spans="1:16">
+      <c r="A135" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="I135" s="1" t="s">
         <v>164</v>
       </c>
+      <c r="J135" s="1" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="136" spans="1:16">
+      <c r="A136" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="I136" s="1" t="s">
         <v>164</v>
       </c>
+      <c r="J136" s="1" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="137" spans="1:16">
+      <c r="A137" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="I137" s="1" t="s">
         <v>164</v>
+      </c>
+      <c r="J137" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16">
+      <c r="A138" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I138" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J138" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16">
+      <c r="A139" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I139" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J139" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16">
+      <c r="A140" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I140" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J140" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16">
+      <c r="A141" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I141" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J141" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16">
+      <c r="A142" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I142" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J142" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16">
+      <c r="A143" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I143" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J143" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16">
+      <c r="A144" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I144" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J144" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10">
+      <c r="A145" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I145" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J145" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10">
+      <c r="A146" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I146" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J146" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating data master sheet
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24660" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="254">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -753,7 +753,37 @@
     <t>74</t>
   </si>
   <si>
-    <t>11:-8</t>
+    <t>2017-1-14</t>
+  </si>
+  <si>
+    <t>10:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changed water 2017-11-15 10:16 </t>
+  </si>
+  <si>
+    <t>2017-11-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 </t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>this individual went directly to free run from the plate (no trikinetics in the room); changed water 2017-11-13 21:36; disturbed to check for deaths 2017-11-15 21:42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disturbed to check for deaths 2017-11-14 10:18; disturbed to check for deathh 2017-11-16 10:02 </t>
   </si>
 </sst>
 </file>
@@ -1474,13 +1504,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W153"/>
+  <dimension ref="A1:W156"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D130" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="O103" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A134" sqref="A134"/>
+      <selection pane="bottomRight" activeCell="Q118" sqref="Q118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4279,7 +4309,7 @@
         <v>183</v>
       </c>
       <c r="W107" s="1" t="s">
-        <v>185</v>
+        <v>252</v>
       </c>
     </row>
     <row r="108" spans="1:23">
@@ -5146,6 +5176,15 @@
       <c r="M133" s="1" t="s">
         <v>201</v>
       </c>
+      <c r="N133" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="O133" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="P133" s="1" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="134" spans="1:16">
       <c r="A134" s="1" t="s">
@@ -5433,7 +5472,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="145" spans="1:15">
+    <row r="145" spans="1:16">
       <c r="A145" s="1" t="s">
         <v>61</v>
       </c>
@@ -5459,7 +5498,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="146" spans="1:15">
+    <row r="146" spans="1:16">
       <c r="A146" s="1" t="s">
         <v>12</v>
       </c>
@@ -5500,7 +5539,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="147" spans="1:15">
+    <row r="147" spans="1:16">
       <c r="A147" s="1" t="s">
         <v>61</v>
       </c>
@@ -5526,7 +5565,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="148" spans="1:15">
+    <row r="148" spans="1:16">
       <c r="A148" s="1" t="s">
         <v>61</v>
       </c>
@@ -5567,7 +5606,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="149" spans="1:15">
+    <row r="149" spans="1:16">
       <c r="A149" s="1" t="s">
         <v>73</v>
       </c>
@@ -5608,7 +5647,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="150" spans="1:15">
+    <row r="150" spans="1:16">
       <c r="A150" s="1" t="s">
         <v>13</v>
       </c>
@@ -5642,8 +5681,11 @@
       <c r="M150" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="151" spans="1:15">
+      <c r="P150" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16">
       <c r="A151" s="1" t="s">
         <v>61</v>
       </c>
@@ -5684,7 +5726,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="152" spans="1:15">
+    <row r="152" spans="1:16">
       <c r="A152" s="1" t="s">
         <v>12</v>
       </c>
@@ -5719,7 +5761,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="153" spans="1:15">
+    <row r="153" spans="1:16">
       <c r="A153" s="1" t="s">
         <v>61</v>
       </c>
@@ -5751,7 +5793,112 @@
         <v>120</v>
       </c>
       <c r="M153" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16">
+      <c r="A154" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I154" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J154" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K154" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="L154" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M154" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16">
+      <c r="A155" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I155" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J155" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K155" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="L155" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M155" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16">
+      <c r="A156" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G156" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I156" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J156" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K156" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L156" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M156" s="1" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data sheet, some scripts that undergrads worked on
dataplay script; kylie and chelsea worked on
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="24500" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="258">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -793,6 +793,9 @@
   </si>
   <si>
     <t>changed water 2017-11-17 10:42; disturbed to check for death 2017-11-17 9:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changed water 2017-11-28 9:59 </t>
   </si>
 </sst>
 </file>
@@ -1528,10 +1531,10 @@
   <dimension ref="A1:W157"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K126" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F126" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S152" sqref="S152"/>
+      <selection pane="bottomRight" activeCell="P154" sqref="P154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5819,6 +5822,9 @@
       <c r="M153" s="1" t="s">
         <v>241</v>
       </c>
+      <c r="P153" s="1" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="154" spans="1:16">
       <c r="A154" s="1" t="s">

</xml_diff>

<commit_message>
Updating eclosion information 2017-12-04
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24500" windowHeight="15360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="285">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -874,6 +874,9 @@
   </si>
   <si>
     <t xml:space="preserve">this individual went directly to free run from the plate (no trikinetics in the room); disturbed to check for death 2017-11-20 </t>
+  </si>
+  <si>
+    <t>changed water 2017-12-04 10:42</t>
   </si>
 </sst>
 </file>
@@ -1609,10 +1612,10 @@
   <dimension ref="A1:W164"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D141" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G141" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A165" sqref="A165"/>
+      <selection pane="bottomRight" activeCell="Q162" sqref="Q162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6137,6 +6140,9 @@
       <c r="M159" s="1" t="s">
         <v>264</v>
       </c>
+      <c r="P159" s="1" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="160" spans="1:16">
       <c r="A160" s="1" t="s">

</xml_diff>

<commit_message>
Updating data sheet 2018-01-09
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="24500" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -909,9 +909,6 @@
     <t xml:space="preserve">20:40 </t>
   </si>
   <si>
-    <t xml:space="preserve">this individual went directly to free run from the plate (no trikinetics in the room); disturbed to check for death 2017-11-20; changed water 2017-11-28 </t>
-  </si>
-  <si>
     <t xml:space="preserve">10:36 </t>
   </si>
   <si>
@@ -946,6 +943,9 @@
   </si>
   <si>
     <t xml:space="preserve">changed water 2017-11-28 9:59; changed water 2017-12-02 10:01; changed water 2017-12-07 9:39 </t>
+  </si>
+  <si>
+    <t>this individual went directly to free run from the plate (no trikinetics in the room); disturbed to check for death 2017-11-20; changed water 2017-11-28;changed water 2017-12-10 20:00</t>
   </si>
 </sst>
 </file>
@@ -958,6 +958,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1681,10 +1682,10 @@
   <dimension ref="A1:W168"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E153" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="O203" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J175" sqref="J175"/>
+      <selection pane="bottomRight" activeCell="R113" sqref="R113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4615,7 +4616,7 @@
         <v>183</v>
       </c>
       <c r="W110" s="1" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
     </row>
     <row r="111" spans="1:23">
@@ -5924,7 +5925,7 @@
         <v>238</v>
       </c>
       <c r="P151" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="152" spans="1:16">
@@ -6000,7 +6001,7 @@
         <v>241</v>
       </c>
       <c r="P153" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="154" spans="1:16">
@@ -6205,7 +6206,7 @@
         <v>257</v>
       </c>
       <c r="P158" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="159" spans="1:16">
@@ -6281,7 +6282,7 @@
         <v>263</v>
       </c>
       <c r="P160" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="161" spans="1:16">
@@ -6363,7 +6364,7 @@
         <v>266</v>
       </c>
       <c r="P162" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="163" spans="1:16">
@@ -6497,7 +6498,7 @@
         <v>31</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>219</v>
@@ -6518,10 +6519,10 @@
         <v>120</v>
       </c>
       <c r="M166" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P166" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="167" spans="1:16">
@@ -6535,10 +6536,10 @@
         <v>70</v>
       </c>
       <c r="D167" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E167" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="E167" s="1" t="s">
-        <v>298</v>
       </c>
       <c r="G167" s="1" t="s">
         <v>111</v>
@@ -6570,10 +6571,10 @@
         <v>115</v>
       </c>
       <c r="D168" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E168" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="G168" s="1" t="s">
         <v>144</v>
@@ -6591,7 +6592,7 @@
         <v>6</v>
       </c>
       <c r="M168" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating trik skipped cohort
No eclosions; just the rearrangement of the tube of a skipped cohort to
enable access to water.
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24500" windowHeight="15360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -942,10 +942,10 @@
     <t>9:29</t>
   </si>
   <si>
-    <t xml:space="preserve">changed water 2017-11-28 9:59; changed water 2017-12-02 10:01; changed water 2017-12-07 9:39 </t>
-  </si>
-  <si>
     <t>this individual went directly to free run from the plate (no trikinetics in the room); disturbed to check for death 2017-11-20; changed water 2017-11-28;changed water 2017-12-10 20:00</t>
+  </si>
+  <si>
+    <t>changed water 2017-11-28 9:59; changed water 2017-12-02 10:01; changed water 2017-12-07 9:39; rearranged position of water tube 2018-01-10 19:20</t>
   </si>
 </sst>
 </file>
@@ -1682,10 +1682,10 @@
   <dimension ref="A1:W168"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="O203" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D134" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R113" sqref="R113"/>
+      <selection pane="bottomRight" activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4616,7 +4616,7 @@
         <v>183</v>
       </c>
       <c r="W110" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="111" spans="1:23">
@@ -6001,7 +6001,7 @@
         <v>241</v>
       </c>
       <c r="P153" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="154" spans="1:16">

</xml_diff>

<commit_message>
Updates to data sheet
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="24500" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="314">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -945,7 +945,25 @@
     <t>this individual went directly to free run from the plate (no trikinetics in the room); disturbed to check for death 2017-11-20; changed water 2017-11-28;changed water 2017-12-10 20:00</t>
   </si>
   <si>
-    <t>changed water 2017-11-28 9:59; changed water 2017-12-02 10:01; changed water 2017-12-07 9:39; rearranged position of water tube 2018-01-10 19:20</t>
+    <t>2018-01-11</t>
+  </si>
+  <si>
+    <t>10:44</t>
+  </si>
+  <si>
+    <t>changed water 2017-11-28 9:59; changed water 2017-12-02 10:01; changed water 2017-12-07 9:39; rearranged position of water tube 2018-01-10 19:20; disturbed to check for death 2018-01-11 10:45</t>
+  </si>
+  <si>
+    <t>2017-11-20</t>
+  </si>
+  <si>
+    <t>11:19</t>
+  </si>
+  <si>
+    <t>2018-01-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:40 </t>
   </si>
 </sst>
 </file>
@@ -1682,10 +1700,10 @@
   <dimension ref="A1:W168"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D134" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E140" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B153" sqref="B153"/>
+      <selection pane="bottomRight" activeCell="O162" sqref="O162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6001,7 +6019,7 @@
         <v>241</v>
       </c>
       <c r="P153" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="154" spans="1:16">
@@ -6243,6 +6261,12 @@
       <c r="M159" s="1" t="s">
         <v>263</v>
       </c>
+      <c r="N159" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="O159" s="1" t="s">
+        <v>313</v>
+      </c>
       <c r="P159" s="1" t="s">
         <v>291</v>
       </c>
@@ -6363,6 +6387,12 @@
       <c r="M162" s="1" t="s">
         <v>266</v>
       </c>
+      <c r="N162" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="O162" s="1" t="s">
+        <v>308</v>
+      </c>
       <c r="P162" s="1" t="s">
         <v>301</v>
       </c>
@@ -6558,6 +6588,12 @@
       </c>
       <c r="M167" s="1" t="s">
         <v>173</v>
+      </c>
+      <c r="N167" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="O167" s="1" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="168" spans="1:16">

</xml_diff>

<commit_message>
2018-01-12 Updating data sheets
Checked for RT eclosions; checked for free run deaths and water need; 3
free run deaths and 1 RT death
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="316">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -964,6 +964,12 @@
   </si>
   <si>
     <t xml:space="preserve">10:40 </t>
+  </si>
+  <si>
+    <t>2018-01-12</t>
+  </si>
+  <si>
+    <t>19:15</t>
   </si>
 </sst>
 </file>
@@ -1700,10 +1706,10 @@
   <dimension ref="A1:W168"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="L140" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O162" sqref="O162"/>
+      <selection pane="bottomRight" activeCell="T157" sqref="T157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6185,6 +6191,12 @@
       <c r="M157" s="1" t="s">
         <v>254</v>
       </c>
+      <c r="N157" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="O157" s="1" t="s">
+        <v>315</v>
+      </c>
       <c r="P157" s="1" t="s">
         <v>292</v>
       </c>

</xml_diff>

<commit_message>
Update to master data sheet 2018-01-15
No eclosions and 1 RT death; 2 free run deaths
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24500" windowHeight="15360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="318">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -970,6 +970,12 @@
   </si>
   <si>
     <t>19:15</t>
+  </si>
+  <si>
+    <t>2018-01-15</t>
+  </si>
+  <si>
+    <t>13:13</t>
   </si>
 </sst>
 </file>
@@ -1706,10 +1712,10 @@
   <dimension ref="A1:W168"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E140" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T157" sqref="T157"/>
+      <selection pane="bottomRight" activeCell="P158" sqref="P158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6235,6 +6241,12 @@
       <c r="M158" s="1" t="s">
         <v>257</v>
       </c>
+      <c r="N158" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="O158" s="1" t="s">
+        <v>317</v>
+      </c>
       <c r="P158" s="1" t="s">
         <v>300</v>
       </c>

</xml_diff>

<commit_message>
2018-01-22 updated cohort treatments and eclosions
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24760" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="322">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -976,6 +976,18 @@
   </si>
   <si>
     <t>13:13</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>2018-01-22</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>13:34</t>
   </si>
 </sst>
 </file>
@@ -1709,13 +1721,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W168"/>
+  <dimension ref="A1:W169"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D140" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P158" sqref="P158"/>
+      <selection pane="bottomRight" activeCell="M170" sqref="M170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6655,6 +6667,41 @@
         <v>305</v>
       </c>
     </row>
+    <row r="169" spans="1:16">
+      <c r="A169" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I169" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J169" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K169" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L169" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M169" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H122"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
2018-02-04 updating data sheets
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24760" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="24180" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="327">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -921,9 +921,6 @@
     <t xml:space="preserve">disturbed to check for death 2017-12-03 </t>
   </si>
   <si>
-    <t xml:space="preserve">changed water 2017-12-05 9:40 </t>
-  </si>
-  <si>
     <t xml:space="preserve">changed water 2017-12-05 9:38 </t>
   </si>
   <si>
@@ -951,9 +948,6 @@
     <t>10:44</t>
   </si>
   <si>
-    <t>changed water 2017-11-28 9:59; changed water 2017-12-02 10:01; changed water 2017-12-07 9:39; rearranged position of water tube 2018-01-10 19:20; disturbed to check for death 2018-01-11 10:45</t>
-  </si>
-  <si>
     <t>2017-11-20</t>
   </si>
   <si>
@@ -988,6 +982,27 @@
   </si>
   <si>
     <t>13:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unknown </t>
+  </si>
+  <si>
+    <t>2018-02-02</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>13:28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changed water 2017-12-05 9:40; distubed to check for death 2018-02-02 12:57; disturbed to check for death 2018-02-04 8:46 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">changed water 2017-11-28 9:59; changed water 2017-12-02 10:01; changed water 2017-12-07 9:39; rearranged position of water tube 2018-01-10 19:20; disturbed to check for death 2018-01-11 10:45; changed water 2018-02-02 13:29 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">changed water 2018-02-02 13:33 </t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1015,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1721,13 +1736,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W169"/>
+  <dimension ref="A1:W170"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F140" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M170" sqref="M170"/>
+      <selection pane="bottomRight" activeCell="P165" sqref="P165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4658,7 +4673,7 @@
         <v>183</v>
       </c>
       <c r="W110" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="111" spans="1:23">
@@ -5967,7 +5982,7 @@
         <v>238</v>
       </c>
       <c r="P151" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="152" spans="1:16">
@@ -6043,7 +6058,7 @@
         <v>241</v>
       </c>
       <c r="P153" s="1" t="s">
-        <v>309</v>
+        <v>325</v>
       </c>
     </row>
     <row r="154" spans="1:16">
@@ -6210,10 +6225,10 @@
         <v>254</v>
       </c>
       <c r="N157" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O157" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P157" s="1" t="s">
         <v>292</v>
@@ -6254,13 +6269,13 @@
         <v>257</v>
       </c>
       <c r="N158" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O158" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="P158" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="159" spans="1:16">
@@ -6298,10 +6313,10 @@
         <v>263</v>
       </c>
       <c r="N159" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="O159" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="P159" s="1" t="s">
         <v>291</v>
@@ -6424,13 +6439,13 @@
         <v>266</v>
       </c>
       <c r="N162" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="O162" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="O162" s="1" t="s">
-        <v>308</v>
-      </c>
       <c r="P162" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="163" spans="1:16">
@@ -6552,6 +6567,9 @@
       <c r="M165" s="1" t="s">
         <v>284</v>
       </c>
+      <c r="P165" s="1" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="166" spans="1:16">
       <c r="A166" s="1" t="s">
@@ -6588,7 +6606,7 @@
         <v>295</v>
       </c>
       <c r="P166" s="1" t="s">
-        <v>299</v>
+        <v>324</v>
       </c>
     </row>
     <row r="167" spans="1:16">
@@ -6626,10 +6644,10 @@
         <v>173</v>
       </c>
       <c r="N167" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="O167" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="168" spans="1:16">
@@ -6643,10 +6661,10 @@
         <v>115</v>
       </c>
       <c r="D168" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E168" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="G168" s="1" t="s">
         <v>144</v>
@@ -6664,7 +6682,7 @@
         <v>6</v>
       </c>
       <c r="M168" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="169" spans="1:16">
@@ -6675,13 +6693,13 @@
         <v>10</v>
       </c>
       <c r="C169" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E169" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="G169" s="1" t="s">
         <v>111</v>
@@ -6699,7 +6717,42 @@
         <v>6</v>
       </c>
       <c r="M169" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16">
+      <c r="A170" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D170" s="1" t="s">
         <v>321</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I170" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J170" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K170" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="L170" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M170" s="1" t="s">
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2018-02-13 so eclosion and column updates
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -918,9 +918,6 @@
     <t>93</t>
   </si>
   <si>
-    <t xml:space="preserve">disturbed to check for death 2017-12-03 </t>
-  </si>
-  <si>
     <t xml:space="preserve">changed water 2017-12-05 9:38 </t>
   </si>
   <si>
@@ -996,9 +993,6 @@
     <t>13:28</t>
   </si>
   <si>
-    <t xml:space="preserve">changed water 2017-12-05 9:40; distubed to check for death 2018-02-02 12:57; disturbed to check for death 2018-02-04 8:46 </t>
-  </si>
-  <si>
     <t xml:space="preserve">changed water 2018-02-02 13:33 </t>
   </si>
   <si>
@@ -1012,6 +1006,12 @@
   </si>
   <si>
     <t>19:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disturbed to check for death 2017-12-03; changed water 2018-02-13 14:02 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">changed water 2017-12-05 9:40; distubed to check for death 2018-02-02 12:57; disturbed to check for death 2018-02-04 8:46; disturbed to check for death 2018-02-13 13:12; changed water 2018-02-13 14:04; changed water 2018-02-13 14:09 </t>
   </si>
 </sst>
 </file>
@@ -1747,10 +1747,10 @@
   <dimension ref="A1:W170"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F153" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F138" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P170" sqref="P170"/>
+      <selection pane="bottomRight" activeCell="P166" sqref="P166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4681,7 +4681,7 @@
         <v>183</v>
       </c>
       <c r="W110" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="111" spans="1:23">
@@ -5990,7 +5990,7 @@
         <v>238</v>
       </c>
       <c r="P151" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="152" spans="1:16">
@@ -6066,7 +6066,7 @@
         <v>241</v>
       </c>
       <c r="P153" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="154" spans="1:16">
@@ -6233,10 +6233,10 @@
         <v>254</v>
       </c>
       <c r="N157" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="O157" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="O157" s="1" t="s">
-        <v>313</v>
       </c>
       <c r="P157" s="1" t="s">
         <v>292</v>
@@ -6277,13 +6277,13 @@
         <v>257</v>
       </c>
       <c r="N158" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="O158" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="O158" s="1" t="s">
-        <v>315</v>
-      </c>
       <c r="P158" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="159" spans="1:16">
@@ -6321,10 +6321,10 @@
         <v>263</v>
       </c>
       <c r="N159" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="O159" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="O159" s="1" t="s">
-        <v>311</v>
       </c>
       <c r="P159" s="1" t="s">
         <v>291</v>
@@ -6365,7 +6365,7 @@
         <v>263</v>
       </c>
       <c r="P160" s="1" t="s">
-        <v>298</v>
+        <v>328</v>
       </c>
     </row>
     <row r="161" spans="1:16">
@@ -6447,13 +6447,13 @@
         <v>266</v>
       </c>
       <c r="N162" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="O162" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="O162" s="1" t="s">
-        <v>307</v>
-      </c>
       <c r="P162" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="163" spans="1:16">
@@ -6576,13 +6576,13 @@
         <v>284</v>
       </c>
       <c r="N165" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="O165" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="P165" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="166" spans="1:16">
@@ -6620,7 +6620,7 @@
         <v>295</v>
       </c>
       <c r="P166" s="1" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
     <row r="167" spans="1:16">
@@ -6658,10 +6658,10 @@
         <v>173</v>
       </c>
       <c r="N167" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="O167" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="O167" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="168" spans="1:16">
@@ -6675,10 +6675,10 @@
         <v>115</v>
       </c>
       <c r="D168" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E168" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="G168" s="1" t="s">
         <v>144</v>
@@ -6696,7 +6696,7 @@
         <v>6</v>
       </c>
       <c r="M168" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="169" spans="1:16">
@@ -6707,13 +6707,13 @@
         <v>10</v>
       </c>
       <c r="C169" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D169" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="D169" s="1" t="s">
+      <c r="E169" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>318</v>
       </c>
       <c r="G169" s="1" t="s">
         <v>111</v>
@@ -6731,7 +6731,7 @@
         <v>6</v>
       </c>
       <c r="M169" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="170" spans="1:16">
@@ -6742,13 +6742,13 @@
         <v>62</v>
       </c>
       <c r="C170" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D170" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="D170" s="1" t="s">
+      <c r="E170" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>322</v>
       </c>
       <c r="G170" s="1" t="s">
         <v>111</v>
@@ -6766,13 +6766,13 @@
         <v>6</v>
       </c>
       <c r="M170" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N170" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="O170" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="O170" s="1" t="s">
-        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2018-02-22 sc water change
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -1008,9 +1008,6 @@
     <t xml:space="preserve">changed water 2017-12-05 9:40; distubed to check for death 2018-02-02 12:57; disturbed to check for death 2018-02-04 8:46; disturbed to check for death 2018-02-13 13:12; changed water 2018-02-13 14:04; changed water 2018-02-13 14:09 </t>
   </si>
   <si>
-    <t xml:space="preserve">changed water 2017-11-28 9:59; changed water 2017-12-02 10:01; changed water 2017-12-07 9:39; rearranged position of water tube 2018-01-10 19:20; disturbed to check for death 2018-01-11 10:45; changed water 2018-02-02 13:29; 2018-02-07 disturbed (alive but inbetween water and cotton) 13:05; 2018-02-16 disturbed 13:19  </t>
-  </si>
-  <si>
     <t>2018-02-15</t>
   </si>
   <si>
@@ -1018,6 +1015,9 @@
   </si>
   <si>
     <t>this individual went directly to free run from the plate (no trikinetics in the room); disturbed to check for death 2017-11-20; changed water 2017-11-28;changed water 2017-12-10 20:00; dsturbed 2018-01-29 20:02; disturbed 2018-02-02 20:03; disturbed 2018-02-10 20:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changed water 2017-11-28 9:59; changed water 2017-12-02 10:01; changed water 2017-12-07 9:39; rearranged position of water tube 2018-01-10 19:20; disturbed to check for death 2018-01-11 10:45; changed water 2018-02-02 13:29; 2018-02-07 disturbed (alive but inbetween water and cotton) 13:05; 2018-02-16 disturbed 13:19; 2018-02-22 changed water 10:47  </t>
   </si>
 </sst>
 </file>
@@ -1753,10 +1753,10 @@
   <dimension ref="A1:W170"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="U92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E152" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z108" sqref="Z108"/>
+      <selection pane="bottomRight" activeCell="J179" sqref="J179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4687,13 +4687,13 @@
         <v>183</v>
       </c>
       <c r="U110" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="V110" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="V110" s="1" t="s">
+      <c r="W110" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="W110" s="1" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="111" spans="1:23">
@@ -6078,7 +6078,7 @@
         <v>241</v>
       </c>
       <c r="P153" s="1" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="154" spans="1:16">

</xml_diff>

<commit_message>
2018-02-25 RT and SO eclosion
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="24500" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="336">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -1018,6 +1018,18 @@
   </si>
   <si>
     <t xml:space="preserve">changed water 2017-11-28 9:59; changed water 2017-12-02 10:01; changed water 2017-12-07 9:39; rearranged position of water tube 2018-01-10 19:20; disturbed to check for death 2018-01-11 10:45; changed water 2018-02-02 13:29; 2018-02-07 disturbed (alive but inbetween water and cotton) 13:05; 2018-02-16 disturbed 13:19; 2018-02-22 changed water 10:47  </t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>18:57</t>
+  </si>
+  <si>
+    <t>2018-02-25</t>
   </si>
 </sst>
 </file>
@@ -1750,13 +1762,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W170"/>
+  <dimension ref="A1:W171"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E152" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D152" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J179" sqref="J179"/>
+      <selection pane="bottomRight" activeCell="E175" sqref="E175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6787,6 +6799,41 @@
         <v>325</v>
       </c>
     </row>
+    <row r="171" spans="1:16">
+      <c r="A171" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="G171" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I171" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J171" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K171" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="L171" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M171" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H122"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
2018-02-26 deaths and RT eclosion
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="339">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -1017,9 +1017,6 @@
     <t>this individual went directly to free run from the plate (no trikinetics in the room); disturbed to check for death 2017-11-20; changed water 2017-11-28;changed water 2017-12-10 20:00; dsturbed 2018-01-29 20:02; disturbed 2018-02-02 20:03; disturbed 2018-02-10 20:01</t>
   </si>
   <si>
-    <t xml:space="preserve">changed water 2017-11-28 9:59; changed water 2017-12-02 10:01; changed water 2017-12-07 9:39; rearranged position of water tube 2018-01-10 19:20; disturbed to check for death 2018-01-11 10:45; changed water 2018-02-02 13:29; 2018-02-07 disturbed (alive but inbetween water and cotton) 13:05; 2018-02-16 disturbed 13:19; 2018-02-22 changed water 10:47  </t>
-  </si>
-  <si>
     <t>156</t>
   </si>
   <si>
@@ -1030,13 +1027,25 @@
   </si>
   <si>
     <t>2018-02-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-02-26 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:49 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">stuck in cotton </t>
+  </si>
+  <si>
+    <t xml:space="preserve">changed water 2017-11-28 9:59; changed water 2017-12-02 10:01; changed water 2017-12-07 9:39; rearranged position of water tube 2018-01-10 19:20; disturbed to check for death 2018-01-11 10:45; changed water 2018-02-02 13:29; 2018-02-07 disturbed (alive but inbetween water and cotton) 13:05; 2018-02-16 disturbed 13:19; 2018-02-22 changed water 10:47; 2018-02-26 changed food 13:25 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1063,6 +1072,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1765,10 +1780,10 @@
   <dimension ref="A1:W171"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D152" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F150" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E175" sqref="E175"/>
+      <selection pane="bottomRight" activeCell="G174" sqref="G174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6090,7 +6105,7 @@
         <v>241</v>
       </c>
       <c r="P153" s="1" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
     </row>
     <row r="154" spans="1:16">
@@ -6807,13 +6822,13 @@
         <v>6</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G171" s="1" t="s">
         <v>144</v>
@@ -6831,11 +6846,21 @@
         <v>6</v>
       </c>
       <c r="M171" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
+      </c>
+      <c r="N171" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="O171" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="P171" s="1" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H122"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
2018-04-09 eclosions and free run update
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="24020" windowHeight="14880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="349">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -1066,6 +1066,9 @@
   </si>
   <si>
     <t xml:space="preserve">changed water 2017-12-05 9:40; distubed to check for death 2018-02-02 12:57; disturbed to check for death 2018-02-04 8:46; disturbed to check for death 2018-02-13 13:12; changed water 2018-02-13 14:04; changed water 2018-02-13 14:09; was dead for a while but didn't remove right away </t>
+  </si>
+  <si>
+    <t xml:space="preserve">changed water 2019-04-09 13:20 </t>
   </si>
 </sst>
 </file>
@@ -1821,10 +1824,10 @@
   <dimension ref="A1:W173"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H146" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G139" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O174" sqref="O174"/>
+      <selection pane="bottomRight" activeCell="O169" sqref="O169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6825,6 +6828,9 @@
       <c r="M169" s="1" t="s">
         <v>317</v>
       </c>
+      <c r="P169" s="1" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="170" spans="1:19">
       <c r="A170" s="1" t="s">

</xml_diff>

<commit_message>
2018-04-19 eclosions and free run transfer
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="24260" windowHeight="15120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="353">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -1075,6 +1075,12 @@
   </si>
   <si>
     <t>19:10</t>
+  </si>
+  <si>
+    <t>2018-04-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">partially eclosed 2018-04-19 </t>
   </si>
 </sst>
 </file>
@@ -1087,6 +1093,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1827,13 +1834,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W174"/>
+  <dimension ref="A1:W175"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D149" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G157" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M175" sqref="M175"/>
+      <selection pane="bottomRight" activeCell="P175" sqref="P175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7051,6 +7058,35 @@
         <v>350</v>
       </c>
     </row>
+    <row r="175" spans="1:19">
+      <c r="A175" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I175" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="J175" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P175" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H122"/>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
2018-04-23 notebook and frre run transfer update
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="24260" windowHeight="15120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="363">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -1081,6 +1081,36 @@
   </si>
   <si>
     <t xml:space="preserve">partially eclosed 2018-04-19 </t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>2018-04-20</t>
+  </si>
+  <si>
+    <t>19:55</t>
+  </si>
+  <si>
+    <t>2018-04-21</t>
+  </si>
+  <si>
+    <t>18:36</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>19:30</t>
+  </si>
+  <si>
+    <t>2018-04-23</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>13:23</t>
   </si>
 </sst>
 </file>
@@ -1152,8 +1182,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="159">
+  <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1346,7 +1392,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="159">
+  <cellStyles count="175">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1426,6 +1472,14 @@
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1505,6 +1559,14 @@
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1834,13 +1896,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W175"/>
+  <dimension ref="A1:W179"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G157" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D157" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P175" sqref="P175"/>
+      <selection pane="bottomRight" activeCell="E171" sqref="E171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6841,6 +6903,12 @@
       <c r="M169" s="1" t="s">
         <v>317</v>
       </c>
+      <c r="N169" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="O169" s="1" t="s">
+        <v>357</v>
+      </c>
       <c r="P169" s="1" t="s">
         <v>348</v>
       </c>
@@ -7085,6 +7153,146 @@
       </c>
       <c r="P175" s="1" t="s">
         <v>352</v>
+      </c>
+    </row>
+    <row r="176" spans="1:19">
+      <c r="A176" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I176" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="J176" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K176" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L176" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M176" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13">
+      <c r="A177" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I177" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="J177" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K177" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L177" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M177" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13">
+      <c r="A178" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G178" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I178" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="J178" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K178" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="L178" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M178" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13">
+      <c r="A179" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I179" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="J179" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K179" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="L179" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M179" s="1" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2018-04-29 eclosions and free run transfer
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="24260" windowHeight="15120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="366">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -1117,6 +1117,9 @@
   </si>
   <si>
     <t>18:47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">helped to remove from water tube entrance 2018-04-29 11:12 </t>
   </si>
 </sst>
 </file>
@@ -1905,10 +1908,10 @@
   <dimension ref="A1:W180"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D157" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F157" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M181" sqref="M181"/>
+      <selection pane="bottomRight" activeCell="N183" sqref="N183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7196,7 +7199,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="177" spans="1:13">
+    <row r="177" spans="1:16">
       <c r="A177" s="1" t="s">
         <v>163</v>
       </c>
@@ -7230,8 +7233,11 @@
       <c r="M177" s="1" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="178" spans="1:13">
+      <c r="P177" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="178" spans="1:16">
       <c r="A178" s="1" t="s">
         <v>163</v>
       </c>
@@ -7266,7 +7272,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="179" spans="1:13">
+    <row r="179" spans="1:16">
       <c r="A179" s="1" t="s">
         <v>163</v>
       </c>
@@ -7301,7 +7307,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="180" spans="1:13">
+    <row r="180" spans="1:16">
       <c r="A180" s="1" t="s">
         <v>163</v>
       </c>

</xml_diff>

<commit_message>
2018-05-03 eclosions and free run transfer
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="24260" windowHeight="15120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="371">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -1126,6 +1126,15 @@
   </si>
   <si>
     <t>19:57</t>
+  </si>
+  <si>
+    <t>2018-05-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:09 </t>
+  </si>
+  <si>
+    <t>eclosed in between cells C/D 9/10</t>
   </si>
 </sst>
 </file>
@@ -1197,8 +1206,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="175">
+  <cellStyleXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1407,7 +1420,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="175">
+  <cellStyles count="179">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1495,6 +1508,8 @@
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1582,6 +1597,8 @@
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1911,13 +1928,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W181"/>
+  <dimension ref="A1:W182"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D154" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="F167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M182" sqref="M182"/>
+      <selection pane="bottomRight" activeCell="O188" sqref="O188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7383,6 +7400,44 @@
         <v>367</v>
       </c>
     </row>
+    <row r="182" spans="1:16">
+      <c r="A182" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G182" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I182" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="J182" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K182" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L182" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M182" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="P182" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H122"/>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
2018-06-17 eclosions and free run transfer update
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylielennon\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AE24BD-E0E9-4E56-A33F-A1059570F4D3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B1EEC9-F75D-46E0-B706-CDD6833516B5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10995" yWindow="10020" windowWidth="24255" windowHeight="15120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="405">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -1231,6 +1231,18 @@
   </si>
   <si>
     <t>2018-06-15</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>2018-06-17</t>
+  </si>
+  <si>
+    <t>13:19</t>
+  </si>
+  <si>
+    <t>290</t>
   </si>
 </sst>
 </file>
@@ -2032,13 +2044,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W194"/>
+  <dimension ref="A1:W195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M167" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D176" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U178" sqref="U178"/>
+      <selection pane="bottomRight" activeCell="G201" sqref="G201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8142,6 +8154,41 @@
         <v>336</v>
       </c>
     </row>
+    <row r="195" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="G195" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I195" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J195" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K195" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L195" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M195" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H122" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
2018-06-26 free run update
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F802C8B-8312-4C24-BF8A-F4114D119219}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C74031-E47C-4002-869D-D1E67C6C8B52}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10995" yWindow="10020" windowWidth="24255" windowHeight="15120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1987" uniqueCount="435">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -1324,6 +1324,15 @@
   </si>
   <si>
     <t>13:00</t>
+  </si>
+  <si>
+    <t>2018-06-26</t>
+  </si>
+  <si>
+    <t>20:05</t>
+  </si>
+  <si>
+    <t>21</t>
   </si>
 </sst>
 </file>
@@ -2128,10 +2137,10 @@
   <dimension ref="A1:W201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D189" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="M165" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C199" sqref="C199"/>
+      <selection pane="bottomRight" activeCell="S195" sqref="S195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8337,6 +8346,24 @@
       <c r="M196" s="1" t="s">
         <v>407</v>
       </c>
+      <c r="N196" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="O196" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="Q196" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="R196" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="S196" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="T196" s="1" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="197" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">

</xml_diff>

<commit_message>
2018-07-05 free run update
</commit_message>
<xml_diff>
--- a/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
+++ b/Data/2017-10-22_skipped_apple_cohort_eclosions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A340DD-10B4-4710-B0A8-4AD814A1ED0C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B312994E-0E17-497E-8895-B8B41BC824CA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10995" yWindow="10020" windowWidth="24255" windowHeight="15120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="437">
   <si>
     <t>Cohort_day</t>
   </si>
@@ -1336,6 +1336,9 @@
   </si>
   <si>
     <t>2018-06-27</t>
+  </si>
+  <si>
+    <t>2018-07-05</t>
   </si>
 </sst>
 </file>
@@ -2143,10 +2146,10 @@
   <dimension ref="A1:W201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="N171" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="N110" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W188" sqref="W188"/>
+      <selection pane="bottomRight" activeCell="U117" sqref="U117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5159,7 +5162,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>13</v>
       </c>
@@ -5182,7 +5185,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>11</v>
       </c>
@@ -5205,7 +5208,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>73</v>
       </c>
@@ -5228,7 +5231,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>61</v>
       </c>
@@ -5251,7 +5254,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>61</v>
       </c>
@@ -5274,7 +5277,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>12</v>
       </c>
@@ -5297,7 +5300,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>61</v>
       </c>
@@ -5320,7 +5323,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>12</v>
       </c>
@@ -5343,7 +5346,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>13</v>
       </c>
@@ -5366,7 +5369,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>13</v>
       </c>
@@ -5389,7 +5392,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A123" s="8" t="s">
         <v>163</v>
       </c>
@@ -5433,7 +5436,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A124" s="8" t="s">
         <v>75</v>
       </c>
@@ -5477,7 +5480,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A125" s="8" t="s">
         <v>163</v>
       </c>
@@ -5521,7 +5524,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
         <v>163</v>
       </c>
@@ -5564,8 +5567,17 @@
       <c r="P126" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U126" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="V126" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="W126" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A127" s="8" t="s">
         <v>163</v>
       </c>
@@ -5609,7 +5621,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
         <v>163</v>
       </c>

</xml_diff>